<commit_message>
Ajout des pages stages, correction carouselle, ajout conversation, et fiche E4
</commit_message>
<xml_diff>
--- a/assets/Tableau de synthèse - ALLAOUAT Abdenour - Epreuve E4.xlsx
+++ b/assets/Tableau de synthèse - ALLAOUAT Abdenour - Epreuve E4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\louisarmand.local\EspacePeda\Eleves_SIO\Eleves\BTS2SIOB\ALLAOUAT_Abdenour_(aallaouat)\Downloads\PORTFOLIO\Site\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdenour Allaouat\Desktop\Porfolios\Portfolio\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF50DB8-A627-4407-8119-A6B14B9B7AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -184,16 +185,26 @@
     <t>25/05/2023
 29/06/2023</t>
   </si>
+  <si>
+    <t>STAGE 2ème année : Création d'une application Windows, premettant de générer une carte interactive de l'ensemble de l'offre de formation de la région académique.</t>
+  </si>
+  <si>
+    <t>08/01/2024
+16/02/2024</t>
+  </si>
+  <si>
+    <t>img\index\conversasion.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -267,6 +278,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -288,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -675,12 +698,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -688,22 +740,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -712,10 +764,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -739,7 +791,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,25 +818,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -793,13 +845,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -823,22 +875,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -862,12 +926,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Euro" xfId="1"/>
+  <cellStyles count="3">
+    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -900,7 +965,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Multiplication 1"/>
+        <xdr:cNvPr id="2" name="Multiplication 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -943,9 +1014,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -983,9 +1054,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1020,7 +1091,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1055,7 +1126,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1228,14 +1299,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BG82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1306,20 +1377,20 @@
       <c r="X2" s="33"/>
     </row>
     <row r="3" spans="1:59" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="16" t="s">
@@ -1339,20 +1410,20 @@
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:59" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="9" t="s">
@@ -1371,38 +1442,38 @@
       <c r="X4" s="42"/>
     </row>
     <row r="5" spans="1:59" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="56"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="60"/>
     </row>
     <row r="6" spans="1:59" ht="141" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="21" t="s">
@@ -1441,8 +1512,8 @@
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="1:59" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="41" t="s">
         <v>19</v>
       </c>
@@ -1731,7 +1802,7 @@
       <c r="A11" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="50">
         <v>45071</v>
       </c>
       <c r="C11" s="26"/>
@@ -1814,7 +1885,7 @@
       <c r="O12" s="43"/>
       <c r="P12" s="43"/>
       <c r="Q12" s="12"/>
-      <c r="R12" s="43"/>
+      <c r="R12" s="12"/>
       <c r="S12" s="44"/>
       <c r="T12" s="44"/>
       <c r="U12" s="45"/>
@@ -1920,30 +1991,36 @@
       <c r="BF13"/>
       <c r="BG13"/>
     </row>
-    <row r="14" spans="1:59" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+    <row r="14" spans="1:59" s="2" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="K14" s="43"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
       <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="12"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="45"/>
       <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
+      <c r="W14" s="65" t="s">
+        <v>48</v>
+      </c>
       <c r="X14" s="34"/>
       <c r="Y14"/>
       <c r="Z14"/>
@@ -1982,30 +2059,30 @@
       <c r="BG14"/>
     </row>
     <row r="15" spans="1:59" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="34"/>
       <c r="Y15"/>
       <c r="Z15"/>
       <c r="AA15"/>
@@ -2043,30 +2120,30 @@
       <c r="BG15"/>
     </row>
     <row r="16" spans="1:59" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="34"/>
       <c r="Y16"/>
       <c r="Z16"/>
       <c r="AA16"/>
@@ -3609,10 +3686,13 @@
     <mergeCell ref="A4:L4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="W14" r:id="rId1" xr:uid="{3FE34BE2-AA96-414F-9BCA-7ACFBEB0C9F3}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>